<commit_message>
finished full pivot for QC and analytes
</commit_message>
<xml_diff>
--- a/data/UWF_yr3_for_SRC.xlsx
+++ b/data/UWF_yr3_for_SRC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://santarosacofl-my.sharepoint.com/personal/michaelf_santarosa_fl_gov/Documents/Projects/Santa Rosa Sound Water Quality/Data/UWF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\wqx-data-upload-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{5E05232D-2CFE-4DA7-94DA-A09B08BC896A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7057522C-5554-4DC3-BC31-C3A3B9C71C81}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9BCC9F-E98C-4CEE-8284-CA23C8F09A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Dissnutrchla" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>JOIN</t>
+  </si>
+  <si>
+    <t>TN_QC</t>
   </si>
 </sst>
 </file>
@@ -3828,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312E3300-7D98-4DE2-8EB4-06D650B5C67C}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,7 +3856,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -5673,7 +5676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C74AA2-AB3C-49BB-BFDE-22E57F8B594D}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
all joins fixed, most analysis dates are available. Just need confirmations of april chla analysis
</commit_message>
<xml_diff>
--- a/data/UWF_yr3_for_SRC.xlsx
+++ b/data/UWF_yr3_for_SRC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\wqx-data-upload-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9BCC9F-E98C-4CEE-8284-CA23C8F09A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9B528-D4A9-43A2-BB21-B25E85EAAD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Dissnutrchla" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -168,10 +168,22 @@
     <t>Present Below Detection limit</t>
   </si>
   <si>
-    <t>JOIN</t>
+    <t>TN_QC</t>
   </si>
   <si>
-    <t>TN_QC</t>
+    <t>DN_JOIN</t>
+  </si>
+  <si>
+    <t>TKNTP_JOIN</t>
+  </si>
+  <si>
+    <t>TNTP_JOIN</t>
+  </si>
+  <si>
+    <t>ENT_JOIN</t>
+  </si>
+  <si>
+    <t>TSS_JOIN</t>
   </si>
 </sst>
 </file>
@@ -626,10 +638,10 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -2957,7 +2969,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H28"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,7 +3001,7 @@
         <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3831,8 +3843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312E3300-7D98-4DE2-8EB4-06D650B5C67C}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,7 +3868,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -3865,7 +3877,7 @@
         <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4532,7 +4544,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4570,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5676,8 +5688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C74AA2-AB3C-49BB-BFDE-22E57F8B594D}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5701,7 +5713,7 @@
         <v>40</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
year 3 WQX upload complete
</commit_message>
<xml_diff>
--- a/data/UWF_yr3_for_SRC.xlsx
+++ b/data/UWF_yr3_for_SRC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\wqx-data-upload-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9B528-D4A9-43A2-BB21-B25E85EAAD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB76627-998F-497E-8C6D-EC6DE117266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8681D0B8-A6F3-4555-92D1-36168C7D7CB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Dissnutrchla" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -100,24 +100,6 @@
   </si>
   <si>
     <t>Color PCU</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>IQ</t>
-  </si>
-  <si>
-    <t>UJ2</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>J2</t>
   </si>
   <si>
     <t>Entero</t>
@@ -184,6 +166,12 @@
   </si>
   <si>
     <t>TSS_JOIN</t>
+  </si>
+  <si>
+    <t>Not Detected</t>
+  </si>
+  <si>
+    <t>Present Below Quantification Limit</t>
   </si>
 </sst>
 </file>
@@ -261,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -299,13 +287,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{9F9992F8-4579-43D5-A863-21373B1B17C9}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{E03B771F-1BDB-4BA2-8284-A7D2B99F8FD5}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -638,15 +672,16 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -663,37 +698,37 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -718,7 +753,7 @@
         <v>0.1742691359715185</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J2" s="5">
         <v>3.484149855907781</v>
@@ -752,7 +787,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H3" s="5">
         <v>1.2130945045415125</v>
@@ -762,7 +797,7 @@
         <v>0.98270893371757906</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L3">
         <v>8.81</v>
@@ -793,7 +828,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H4" s="5">
         <v>0.80139440412615803</v>
@@ -803,7 +838,7 @@
         <v>0.62536023054755041</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L4">
         <v>7.67</v>
@@ -830,13 +865,13 @@
         <v>0.35875533862112879</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F5" s="5">
         <v>0.18599592405878018</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H5" s="5">
         <v>0.78545917202975946</v>
@@ -846,7 +881,7 @@
         <v>0.26801152737752165</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L5">
         <v>10.09</v>
@@ -877,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H6" s="5">
         <v>5.8432978456342139</v>
@@ -887,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>4.82</v>
@@ -918,7 +953,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H7" s="5">
         <v>3.3990568944269475</v>
@@ -956,7 +991,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H8" s="5">
         <v>3.646672029759459</v>
@@ -994,7 +1029,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H9" s="5">
         <v>0.71948171984116105</v>
@@ -1004,7 +1039,7 @@
         <v>0.98270893371757906</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>9.68</v>
@@ -1035,7 +1070,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H10" s="5">
         <v>4.9731702724907567</v>
@@ -1073,19 +1108,19 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H11" s="5">
         <v>8.446871148842976E-3</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L11">
         <v>7.62</v>
@@ -1116,7 +1151,7 @@
         <v>0.18599592405878018</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H12" s="5">
         <v>1.4136427951983204</v>
@@ -1126,7 +1161,7 @@
         <v>0.98270893371757906</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L12">
         <v>9.11</v>
@@ -1157,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H13" s="5">
         <v>4.1970565749235469</v>
@@ -1167,7 +1202,7 @@
         <v>0.62536023054755041</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L13">
         <v>8.49</v>
@@ -1270,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H16" s="5">
         <v>7.4189837047167675</v>
@@ -1280,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L16" s="5">
         <v>9.4366049715677498</v>
@@ -1312,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H17" s="5">
         <v>4.1827334656497515</v>
@@ -1322,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L17" s="5">
         <v>15.852209044917473</v>
@@ -1354,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H18" s="5">
         <v>1.8309941719212786</v>
@@ -1364,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L18" s="5">
         <v>3.9546998390643027</v>
@@ -1396,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H19" s="5">
         <v>7.9318210385453707</v>
@@ -1435,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H20" s="5">
         <v>1.6249434574365713</v>
@@ -1445,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L20" s="5">
         <v>8.1179827904840121</v>
@@ -1477,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H21" s="5">
         <v>1.6897614208875393</v>
@@ -1487,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L21" s="5">
         <v>7.3403338118961674</v>
@@ -1519,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H22" s="5">
         <v>6.9293170095800765</v>
@@ -1529,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L22" s="5">
         <v>2.096404871836826</v>
@@ -1561,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H23" s="5">
         <v>16.654082388677423</v>
@@ -1571,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L23" s="5">
         <v>1.9104453334788634</v>
@@ -1603,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H24" s="5">
         <v>4.7470662209207672</v>
@@ -1613,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L24" s="5">
         <v>5.0073868761326317</v>
@@ -1645,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H25" s="5">
         <v>1.8684077354893558</v>
@@ -1655,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L25" s="5">
         <v>2.25180462591918</v>
@@ -1687,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H26" s="5">
         <v>4.1974826011030961</v>
@@ -1697,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L26" s="5">
         <v>1.8720830510903326</v>
@@ -1729,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H27" s="5">
         <v>5.2035531136803543</v>
@@ -1739,7 +1774,7 @@
         <v>0.38589211618257224</v>
       </c>
       <c r="K27" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L27" s="5">
         <v>2.2927677410120184</v>
@@ -1816,7 +1851,7 @@
         <v>0.6</v>
       </c>
       <c r="K29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L29" s="5">
         <v>3.0495511974422196</v>
@@ -1844,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F30" s="5">
         <v>1.5</v>
@@ -1883,13 +1918,13 @@
         <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F31" s="5">
         <v>0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H31" s="5">
         <v>3.5311843096524029</v>
@@ -1899,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L31" s="5">
         <v>1.489495614293713</v>
@@ -1927,13 +1962,13 @@
         <v>2.4387096774193573</v>
       </c>
       <c r="E32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F32" s="5">
         <v>0.6</v>
       </c>
       <c r="G32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H32" s="5">
         <v>10.011490648670039</v>
@@ -1943,7 +1978,7 @@
         <v>0.8999999999999998</v>
       </c>
       <c r="K32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L32" s="5">
         <v>6.9574670089712258</v>
@@ -1971,13 +2006,13 @@
         <v>0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F33" s="5">
         <v>0.6</v>
       </c>
       <c r="G33" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H33" s="5">
         <v>1.8374523413484252</v>
@@ -1987,7 +2022,7 @@
         <v>0.29999999999999977</v>
       </c>
       <c r="K33" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L33" s="5">
         <v>1.394112035696405</v>
@@ -2015,13 +2050,13 @@
         <v>1.3548387096774206</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F34" s="5">
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H34" s="5">
         <v>1.7791915662300106</v>
@@ -2031,7 +2066,7 @@
         <v>0.8999999999999998</v>
       </c>
       <c r="K34" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L34" s="5">
         <v>2.0655449671583987</v>
@@ -2059,13 +2094,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F35" s="5">
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H35" s="5">
         <v>1.480938540854672</v>
@@ -2075,7 +2110,7 @@
         <v>1.2</v>
       </c>
       <c r="K35" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L35" s="5">
         <v>1.1756105570235929</v>
@@ -2103,13 +2138,13 @@
         <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F36" s="5">
         <v>0.6</v>
       </c>
       <c r="G36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H36" s="5">
         <v>1.2009102212012541</v>
@@ -2119,7 +2154,7 @@
         <v>1.4999999999999998</v>
       </c>
       <c r="K36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L36" s="5">
         <v>1.2949805758182593</v>
@@ -2147,13 +2182,13 @@
         <v>0.81290322580645236</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F37" s="5">
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H37" s="5">
         <v>7.9119731662477308</v>
@@ -2163,7 +2198,7 @@
         <v>0.6</v>
       </c>
       <c r="K37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L37" s="5">
         <v>1.1990348150288261</v>
@@ -2191,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F38" s="5">
         <v>0.6</v>
       </c>
       <c r="G38" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H38" s="5">
         <v>1.1012235467296927</v>
@@ -2207,13 +2242,13 @@
         <v>0</v>
       </c>
       <c r="K38" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="L38" s="5">
         <v>7.110994356085415E-2</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="N38" s="5">
         <v>8.2023681377825604</v>
@@ -2237,13 +2272,13 @@
         <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F39" s="5">
         <v>0.6</v>
       </c>
       <c r="G39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H39" s="5">
         <v>2.4407057923725306</v>
@@ -2253,7 +2288,7 @@
         <v>0.6</v>
       </c>
       <c r="K39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L39" s="5">
         <v>1.1810449848808069</v>
@@ -2281,13 +2316,13 @@
         <v>0.81290322580645236</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F40" s="5">
         <v>0.6</v>
       </c>
       <c r="G40" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H40" s="5">
         <v>5.851707171794776</v>
@@ -2297,7 +2332,7 @@
         <v>1.2</v>
       </c>
       <c r="K40" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L40" s="5">
         <v>1.4795637288994945</v>
@@ -2366,7 +2401,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H42" s="5">
         <v>41.27309277995613</v>
@@ -2405,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H43" s="5">
         <v>8.1254464308365524</v>
@@ -2444,7 +2479,7 @@
         <v>0.16374269005847955</v>
       </c>
       <c r="G44" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H44" s="5">
         <v>12.798774437164576</v>
@@ -2479,13 +2514,13 @@
         <v>2.6868908115211849</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F45" s="5">
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H45" s="5">
         <v>6.1269953258484868</v>
@@ -2495,7 +2530,7 @@
         <v>0.926910299003322</v>
       </c>
       <c r="K45" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L45" s="5">
         <v>1.8148916332225273</v>
@@ -2523,13 +2558,13 @@
         <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F46" s="5">
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H46" s="5">
         <v>8.2901136838798593</v>
@@ -2564,13 +2599,13 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F47" s="5">
         <v>0.16374269005847955</v>
       </c>
       <c r="G47" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H47" s="5">
         <v>2.2353669873525317</v>
@@ -2605,13 +2640,13 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F48" s="5">
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H48" s="5">
         <v>9.8250092637280648</v>
@@ -2646,13 +2681,13 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F49" s="5">
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H49" s="5">
         <v>1.2495170861987899</v>
@@ -2687,13 +2722,13 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F50" s="5">
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H50" s="5">
         <v>1.3326424837153299</v>
@@ -2728,13 +2763,13 @@
         <v>2.0505968678129376</v>
       </c>
       <c r="E51" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F51" s="5">
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H51" s="5">
         <v>3.1527234189752464</v>
@@ -2744,7 +2779,7 @@
         <v>1.338870431893687</v>
       </c>
       <c r="K51" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L51" s="5">
         <v>2.3226611598019931</v>
@@ -2776,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H52" s="5">
         <v>1.96042187014136</v>
@@ -2786,7 +2821,7 @@
         <v>0.926910299003322</v>
       </c>
       <c r="K52" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L52" s="5">
         <v>2.2577208437310214</v>
@@ -2818,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H53" s="5">
         <v>4.5807826992466953</v>
@@ -2828,7 +2863,7 @@
         <v>0.926910299003322</v>
       </c>
       <c r="K53" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L53" s="5">
         <v>2.6085180725683852</v>
@@ -2856,13 +2891,13 @@
         <v>0.77800898039644739</v>
       </c>
       <c r="E54" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F54" s="5">
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H54" s="5">
         <v>4.9401411614594224</v>
@@ -2938,7 +2973,7 @@
         <v>0.16374269005847955</v>
       </c>
       <c r="G56" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H56" s="5">
         <v>17.470518901502828</v>
@@ -2969,13 +3004,15 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2989,19 +3026,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3018,14 +3055,12 @@
         <v>0.32</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F2" s="10">
         <v>0.11</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="G2" s="8"/>
       <c r="H2" t="str">
         <f>_xlfn.CONCAT(C2,A2,B2,)</f>
         <v>45580AK41S</v>
@@ -3045,13 +3080,13 @@
         <v>0.33</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>22</v>
+      <c r="G3" t="s">
+        <v>43</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H28" si="0">_xlfn.CONCAT(C3,A3,B3,)</f>
@@ -3072,13 +3107,13 @@
         <v>0.3</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F4" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>23</v>
+      <c r="G4" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3099,13 +3134,13 @@
         <v>0.37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F5" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3129,8 +3164,8 @@
       <c r="F6" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>24</v>
+      <c r="G6" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3151,13 +3186,13 @@
         <v>0.42</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F7" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3178,13 +3213,13 @@
         <v>0.31</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F8" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3205,13 +3240,13 @@
         <v>0.36</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F9" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>24</v>
+      <c r="G9" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3232,13 +3267,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F10" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3259,13 +3294,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F11" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3286,13 +3321,13 @@
         <v>0.3</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F12" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -3313,13 +3348,13 @@
         <v>0.24</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F13" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -3340,13 +3375,13 @@
         <v>0.25</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F14" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3367,13 +3402,13 @@
         <v>0.26</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F15" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -3394,13 +3429,13 @@
         <v>0.42</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F16" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -3421,13 +3456,13 @@
         <v>0.22</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F17" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -3448,13 +3483,13 @@
         <v>0.32</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F18" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -3475,13 +3510,13 @@
         <v>0.24</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F19" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -3502,13 +3537,13 @@
         <v>0.26</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F20" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -3529,13 +3564,13 @@
         <v>0.22</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F21" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -3556,13 +3591,13 @@
         <v>0.25</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F22" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -3583,13 +3618,13 @@
         <v>0.22</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F23" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -3610,13 +3645,13 @@
         <v>0.2</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F24" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -3637,13 +3672,13 @@
         <v>0.23</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F25" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -3664,13 +3699,13 @@
         <v>0.2</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F26" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -3691,13 +3726,13 @@
         <v>0.21</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F27" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -3718,13 +3753,13 @@
         <v>0.2</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F28" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -3835,6 +3870,26 @@
     <sortCondition ref="A2:A55"/>
     <sortCondition descending="1" ref="B2:B55"/>
   </sortState>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>$S3="Present Above Quantification Limit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$S3="Present Below Quantification Limit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>$S3="Not Detected"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+      <formula>$S3="Present Above Quantification Limit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+      <formula>$S3="Present Below Quantification Limit"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+      <formula>$S3="Not Detected"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3844,7 +3899,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3852,6 +3907,7 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3865,19 +3921,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3897,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H2" t="str">
         <f>_xlfn.CONCAT(C2,A2,B2)</f>
@@ -3921,7 +3977,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H29" si="0">_xlfn.CONCAT(C3,A3,B3)</f>
@@ -3945,7 +4001,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3969,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3993,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -4017,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -4041,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -4065,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -4089,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -4113,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -4137,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -4161,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -4185,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -4230,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -4275,7 +4331,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -4320,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -4365,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -4389,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -4413,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -4437,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -4461,7 +4517,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -4485,7 +4541,7 @@
         <v>3.3186695281533229E-3</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -4543,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF20A81-D11D-4A5F-8B9A-3C517B54EC20}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4564,13 +4620,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4625,7 +4681,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -4646,7 +4702,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -4667,7 +4723,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -4688,7 +4744,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -4709,7 +4765,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -4730,7 +4786,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -4770,7 +4826,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -4810,7 +4866,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -4831,7 +4887,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -4852,7 +4908,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -4892,7 +4948,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -4913,7 +4969,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -4934,7 +4990,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -4955,7 +5011,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -4995,7 +5051,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -5054,7 +5110,7 @@
         <v>10</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -5075,7 +5131,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -5095,9 +5151,7 @@
       <c r="D27" s="11">
         <v>41</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="E27" s="11"/>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
         <v>45671AI31S</v>
@@ -5117,7 +5171,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -5195,7 +5249,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -5216,7 +5270,7 @@
         <v>10</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -5237,7 +5291,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -5277,7 +5331,7 @@
         <v>10</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -5298,7 +5352,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -5319,7 +5373,7 @@
         <v>10</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -5378,7 +5432,7 @@
         <v>10</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -5399,7 +5453,7 @@
         <v>10</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -5420,7 +5474,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -5459,7 +5513,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -5480,7 +5534,7 @@
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -5537,7 +5591,7 @@
         <v>10</v>
       </c>
       <c r="E49" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
@@ -5558,7 +5612,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
@@ -5579,7 +5633,7 @@
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
@@ -5636,7 +5690,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
@@ -5688,7 +5742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C74AA2-AB3C-49BB-BFDE-22E57F8B594D}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -5701,19 +5755,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>